<commit_message>
changes with revision of paper
</commit_message>
<xml_diff>
--- a/questionnaires_and_descriptives/tables and figures/EFPTest_feasibility_sample_characteristics.xlsx
+++ b/questionnaires_and_descriptives/tables and figures/EFPTest_feasibility_sample_characteristics.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92d2b1c231d7636d/Desktop/EFP descriptives table - code and data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Projects\EFPTest\Data_analysis\open_materials_code_data_clinical_study\questionnaires_and_descriptives\tables and figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_AD4DB114E441178AC67DF4A44650EED2683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85CB9D38-2D29-4BBC-82B0-DC34CB7AA12D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10548"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="94">
   <si>
     <t>treatment</t>
   </si>
@@ -330,15 +329,19 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>-1,0455</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -515,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -755,10 +758,13 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard_Sample_Descr" xfId="1" xr:uid="{2099B7FF-C83C-4137-8994-928C114A8FBE}"/>
+    <cellStyle name="Standard_Sample_Descr" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1039,29 +1045,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="A30" sqref="A30:J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.73046875" customWidth="1"/>
+    <col min="1" max="1" width="32.77734375" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="5.86328125" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="6.796875" customWidth="1"/>
-    <col min="9" max="9" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.59765625" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" customWidth="1"/>
+    <col min="9" max="9" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" customWidth="1"/>
     <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -1077,7 +1083,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="5"/>
@@ -1091,7 +1097,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="89" t="s">
         <v>0</v>
@@ -1113,7 +1119,7 @@
       <c r="K3" s="91"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -1127,7 +1133,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -1149,7 +1155,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
@@ -1171,7 +1177,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1205,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>12</v>
       </c>
@@ -1221,8 +1227,8 @@
       <c r="G8" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="30">
-        <v>-1.0455000000000001</v>
+      <c r="H8" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="I8" s="31">
         <v>27.86</v>
@@ -1233,7 +1239,7 @@
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>14</v>
       </c>
@@ -1249,7 +1255,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>15</v>
       </c>
@@ -1283,7 +1289,7 @@
       <c r="K10" s="27"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>18</v>
       </c>
@@ -1317,7 +1323,7 @@
       <c r="K11" s="27"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>23</v>
       </c>
@@ -1351,7 +1357,7 @@
       <c r="K12" s="44"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>26</v>
       </c>
@@ -1385,7 +1391,7 @@
       <c r="K13" s="27"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>28</v>
       </c>
@@ -1419,7 +1425,7 @@
       <c r="K14" s="27"/>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>30</v>
       </c>
@@ -1453,7 +1459,7 @@
       <c r="K15" s="27"/>
       <c r="L15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
         <v>31</v>
       </c>
@@ -1469,7 +1475,7 @@
       <c r="K16" s="27"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="50" t="s">
         <v>32</v>
       </c>
@@ -1503,7 +1509,7 @@
       <c r="K17" s="27"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="50" t="s">
         <v>37</v>
       </c>
@@ -1537,7 +1543,7 @@
       <c r="K18" s="27"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="50" t="s">
         <v>42</v>
       </c>
@@ -1571,7 +1577,7 @@
       <c r="K19" s="27"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="50" t="s">
         <v>44</v>
       </c>
@@ -1605,7 +1611,7 @@
       <c r="K20" s="27"/>
       <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="50" t="s">
         <v>47</v>
       </c>
@@ -1639,7 +1645,7 @@
       <c r="K21" s="27"/>
       <c r="L21" s="7"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="50" t="s">
         <v>49</v>
       </c>
@@ -1673,7 +1679,7 @@
       <c r="K22" s="27"/>
       <c r="L22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="50" t="s">
         <v>50</v>
       </c>
@@ -1707,7 +1713,7 @@
       <c r="K23" s="27"/>
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="50" t="s">
         <v>51</v>
       </c>
@@ -1741,7 +1747,7 @@
       <c r="K24" s="27"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B25" s="52"/>
       <c r="C25" s="53"/>
       <c r="D25" s="54"/>
@@ -1754,7 +1760,7 @@
       <c r="K25" s="27"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="82" t="s">
         <v>73</v>
       </c>
@@ -1778,7 +1784,7 @@
       <c r="K26" s="94"/>
       <c r="L26" s="7"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="55" t="s">
         <v>8</v>
       </c>
@@ -1800,7 +1806,7 @@
       <c r="K27" s="59"/>
       <c r="L27" s="59"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="60" t="s">
         <v>54</v>
       </c>
@@ -1834,7 +1840,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="57" t="s">
         <v>92</v>
       </c>
@@ -1853,8 +1859,8 @@
       <c r="F29" s="29">
         <v>38.724139999999998</v>
       </c>
-      <c r="G29" s="29">
-        <v>10.79317</v>
+      <c r="G29" s="95">
+        <v>10.79</v>
       </c>
       <c r="H29" s="67">
         <v>-3.8474309999999998E-2</v>
@@ -1868,7 +1874,7 @@
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="68" t="s">
         <v>56</v>
       </c>
@@ -1884,7 +1890,7 @@
       <c r="K30" s="27"/>
       <c r="L30" s="7"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="70" t="s">
         <v>92</v>
       </c>
@@ -1918,7 +1924,7 @@
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="71" t="s">
         <v>57</v>
       </c>
@@ -1934,7 +1940,7 @@
       <c r="K32" s="27"/>
       <c r="L32" s="7"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="72" t="s">
         <v>92</v>
       </c>
@@ -1968,7 +1974,7 @@
       <c r="K33" s="47"/>
       <c r="L33" s="27"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="70" t="s">
         <v>58</v>
       </c>
@@ -2002,7 +2008,7 @@
       <c r="K34" s="47"/>
       <c r="L34" s="27"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="70" t="s">
         <v>59</v>
       </c>
@@ -2036,7 +2042,7 @@
       <c r="K35" s="47"/>
       <c r="L35" s="27"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="70" t="s">
         <v>60</v>
       </c>
@@ -2070,7 +2076,7 @@
       <c r="K36" s="47"/>
       <c r="L36" s="27"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="70" t="s">
         <v>61</v>
       </c>
@@ -2104,7 +2110,7 @@
       <c r="K37" s="47"/>
       <c r="L37" s="27"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="70" t="s">
         <v>62</v>
       </c>
@@ -2138,7 +2144,7 @@
       <c r="K38" s="47"/>
       <c r="L38" s="27"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="70" t="s">
         <v>63</v>
       </c>
@@ -2172,7 +2178,7 @@
       <c r="K39" s="47"/>
       <c r="L39" s="27"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="45" t="s">
         <v>64</v>
       </c>
@@ -2188,7 +2194,7 @@
       <c r="K40" s="27"/>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="70" t="s">
         <v>92</v>
       </c>
@@ -2222,7 +2228,7 @@
       <c r="K41" s="75"/>
       <c r="L41" s="27"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="70" t="s">
         <v>65</v>
       </c>
@@ -2256,7 +2262,7 @@
       <c r="K42" s="47"/>
       <c r="L42" s="27"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="70" t="s">
         <v>66</v>
       </c>
@@ -2290,7 +2296,7 @@
       <c r="K43" s="47"/>
       <c r="L43" s="27"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="70" t="s">
         <v>67</v>
       </c>
@@ -2324,7 +2330,7 @@
       <c r="K44" s="47"/>
       <c r="L44" s="27"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="70"/>
       <c r="B45" s="50"/>
       <c r="C45" s="50"/>
@@ -2338,7 +2344,7 @@
       <c r="K45" s="47"/>
       <c r="L45" s="27"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="77" t="s">
         <v>8</v>
       </c>
@@ -2360,7 +2366,7 @@
       <c r="K46" s="47"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="78" t="s">
         <v>68</v>
       </c>
@@ -2394,7 +2400,7 @@
       <c r="K47" s="75"/>
       <c r="L47" s="7"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="27" t="s">
         <v>70</v>
       </c>
@@ -2410,7 +2416,7 @@
       <c r="K48" s="75"/>
       <c r="L48" s="27"/>
     </row>
-    <row r="49" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="88" t="s">
         <v>71</v>
       </c>

</xml_diff>